<commit_message>
Changed 'coder' to 'preprint_ID' in codesheet
</commit_message>
<xml_diff>
--- a/template_input_extracted_values.xlsx
+++ b/template_input_extracted_values.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u237972\Desktop\round3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u237972\Git\Screening-for-Statistical-Inconsistencies-in-COVID-19-Preprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,9 +20,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <si>
-    <t xml:space="preserve">Coder: </t>
-  </si>
   <si>
     <t>perc_ratio</t>
   </si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>comparison</t>
+  </si>
+  <si>
+    <t>preprint_ID:</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <dimension ref="A1:AK1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -465,34 +465,34 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
       <c r="K1" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
@@ -516,115 +516,115 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="X2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Moved 'comparison' column in codesheet
</commit_message>
<xml_diff>
--- a/template_input_extracted_values.xlsx
+++ b/template_input_extracted_values.xlsx
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -224,6 +224,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -454,12 +457,14 @@
   <dimension ref="A1:AK1002"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="37" width="14.42578125" style="5"/>
+    <col min="1" max="9" width="14.42578125" style="5"/>
+    <col min="10" max="10" width="14.42578125" style="7"/>
+    <col min="11" max="37" width="14.42578125" style="5"/>
     <col min="38" max="16384" width="14.42578125" style="3"/>
   </cols>
   <sheetData>
@@ -469,28 +474,28 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="7" t="s">
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="8" t="s">
         <v>2</v>
       </c>
+      <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
       <c r="R1" s="2" t="s">
         <v>5</v>
       </c>
@@ -522,28 +527,28 @@
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>3</v>
@@ -628,7 +633,7 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="D3" s="6"/>
+      <c r="C3" s="6"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
@@ -22632,9 +22637,9 @@
   <sheetProtection sheet="1" scenarios="1"/>
   <mergeCells count="4">
     <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>